<commit_message>
MVP1 - mock reply
</commit_message>
<xml_diff>
--- a/doc/MVP1/mvp1 - intents.xlsx
+++ b/doc/MVP1/mvp1 - intents.xlsx
@@ -13,22 +13,140 @@
   </bookViews>
   <sheets>
     <sheet name="intents" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Calendar events</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Intent</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Personalised ?</t>
+  </si>
+  <si>
+    <t>Intent Variation</t>
+  </si>
+  <si>
+    <t>Opponent team</t>
+  </si>
+  <si>
+    <t>My Team</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Match date</t>
+  </si>
+  <si>
+    <t>Match location</t>
+  </si>
+  <si>
+    <t>Match Score</t>
+  </si>
+  <si>
+    <t>Match Referee</t>
+  </si>
+  <si>
+    <t>Get official score</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Wat was de eindscore van FC Dender - Zulte-Waregem ?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Get match location</t>
+  </si>
+  <si>
+    <t>Waar speelt FC Dender volgende zaterdag ?</t>
+  </si>
+  <si>
+    <t>Get referee name</t>
+  </si>
+  <si>
+    <t>Wie fluit de match FC Dender - Zulte-Waregem ?</t>
+  </si>
+  <si>
+    <t>Get match kickoff time</t>
+  </si>
+  <si>
+    <t>Wanneer start de match FC Dender - Zulte-Waregem ?</t>
+  </si>
+  <si>
+    <t>Get match opposite team name</t>
+  </si>
+  <si>
+    <t>Tegen wie speelt FC Dender U9 hun volgende match ?</t>
+  </si>
+  <si>
+    <t>Get player selection status</t>
+  </si>
+  <si>
+    <t>Is Brecht De Wachter geselecteerd voor de match tegen FC Dender ?</t>
+  </si>
+  <si>
+    <t>Get my selection status</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Ben ik geselecteerd voor de match tegen FC Dender ?</t>
+  </si>
+  <si>
+    <t>Get score</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Quel est le score du match de FC Dender</t>
+  </si>
+  <si>
+    <t>Quel est le score du match de FC Dender de ce weekend</t>
+  </si>
+  <si>
+    <t>Quel est le résultat du match FC Dender contre Zulte-Waregem</t>
+  </si>
+  <si>
+    <t>Donne moi le score du match de FC Dender</t>
+  </si>
+  <si>
+    <t>Donne moi le score du dernier match de FC Dender</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>résultat</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +281,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF3C78D8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +482,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -460,6 +604,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -505,8 +664,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -856,17 +1030,534 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="64.5703125" customWidth="1"/>
+    <col min="6" max="12" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+    </row>
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>